<commit_message>
Updated 2020 Dates Files
Updated 2020 Dates Files
</commit_message>
<xml_diff>
--- a/2020/2020FSAdates.xlsx
+++ b/2020/2020FSAdates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robert.thomas\Dropbox\Competitions\2020\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92D6EA30-AF7B-41EA-8573-09A93482D368}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{542A29DF-BC16-46CA-90DB-AE194ADCE026}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1065" yWindow="-15225" windowWidth="27105" windowHeight="13680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="55">
   <si>
     <t>Date</t>
   </si>
@@ -186,6 +188,24 @@
   </si>
   <si>
     <t>OT</t>
+  </si>
+  <si>
+    <t>40255</t>
+  </si>
+  <si>
+    <t>40256</t>
+  </si>
+  <si>
+    <t>40257</t>
+  </si>
+  <si>
+    <t>40258</t>
+  </si>
+  <si>
+    <t>40284</t>
+  </si>
+  <si>
+    <t>40285</t>
   </si>
 </sst>
 </file>
@@ -301,11 +321,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:I96" tableType="xml" totalsRowShown="0" connectionId="2">
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I96">
-    <sortCondition ref="A2:A96"/>
-    <sortCondition ref="F2:F96"/>
-    <sortCondition ref="B2:B96"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:I97" tableType="xml" totalsRowShown="0" connectionId="2">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I97">
+    <sortCondition ref="A2:A97"/>
+    <sortCondition ref="F2:F97"/>
+    <sortCondition ref="B2:B97"/>
   </sortState>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="Date" name="Date">
@@ -637,7 +657,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L96"/>
+  <dimension ref="A1:L97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2480,10 +2500,10 @@
         <v>12</v>
       </c>
       <c r="D52">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E52">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F52" s="1" t="s">
         <v>32</v>
@@ -2497,11 +2517,11 @@
       <c r="I52" s="1"/>
       <c r="K52" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>N/A</v>
+        <v>20200726OE</v>
       </c>
       <c r="L52" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v/>
+        <v>N/A</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
@@ -2512,19 +2532,19 @@
         <v>18</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D53">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E53">
         <v>1</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="H53" s="1" t="s">
         <v>19</v>
@@ -2532,11 +2552,11 @@
       <c r="I53" s="1"/>
       <c r="K53" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>N/A</v>
+        <v>20200726OME</v>
       </c>
       <c r="L53" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v/>
+        <v>20200726OWE</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
@@ -2544,16 +2564,16 @@
         <v>20200726</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F54" s="1" t="s">
         <v>37</v>
@@ -2567,11 +2587,11 @@
       <c r="I54" s="1"/>
       <c r="K54" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>N/A</v>
+        <v>20200726OS</v>
       </c>
       <c r="L54" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v/>
+        <v>N/A</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
@@ -2579,7 +2599,7 @@
         <v>20200726</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>11</v>
@@ -2591,10 +2611,10 @@
         <v>1</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H55" s="1" t="s">
         <v>19</v>
@@ -2614,16 +2634,16 @@
         <v>20200726</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F56" s="1" t="s">
         <v>38</v>
@@ -2637,11 +2657,11 @@
       <c r="I56" s="1"/>
       <c r="K56" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>N/A</v>
+        <v>20200726OF</v>
       </c>
       <c r="L56" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v/>
+        <v>N/A</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
@@ -2652,13 +2672,13 @@
         <v>9</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D57">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E57">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F57" s="1" t="s">
         <v>38</v>
@@ -2672,34 +2692,34 @@
       <c r="I57" s="1"/>
       <c r="K57" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>N/A</v>
+        <v>20200726VE</v>
       </c>
       <c r="L57" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v/>
+        <v>N/A</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>20200816</v>
+        <v>20200726</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E58">
         <v>1</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="H58" s="1" t="s">
         <v>19</v>
@@ -2707,11 +2727,11 @@
       <c r="I58" s="1"/>
       <c r="K58" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20200816U1720MF</v>
+        <v>N/A</v>
       </c>
       <c r="L58" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20200816U1720WF</v>
+        <v/>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
@@ -2719,10 +2739,10 @@
         <v>20200816</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D59">
         <v>0</v>
@@ -2731,22 +2751,24 @@
         <v>1</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H59" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I59" s="1"/>
+      <c r="I59" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="K59" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20200816OBME</v>
+        <v>20200816U1720MF</v>
       </c>
       <c r="L59" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20200816OBWE</v>
+        <v>20200816U1720WF</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
@@ -2754,10 +2776,10 @@
         <v>20200816</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D60">
         <v>0</v>
@@ -2766,10 +2788,10 @@
         <v>1</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H60" s="1" t="s">
         <v>19</v>
@@ -2777,11 +2799,11 @@
       <c r="I60" s="1"/>
       <c r="K60" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20200816U1720MS</v>
+        <v>20200816OBME</v>
       </c>
       <c r="L60" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20200816U1720WS</v>
+        <v>20200816OBWE</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.25">
@@ -2789,10 +2811,10 @@
         <v>20200816</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D61">
         <v>0</v>
@@ -2801,10 +2823,10 @@
         <v>1</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H61" s="1" t="s">
         <v>19</v>
@@ -2812,11 +2834,11 @@
       <c r="I61" s="1"/>
       <c r="K61" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20200816OBMF</v>
+        <v>20200816U1720MS</v>
       </c>
       <c r="L61" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20200816OBWF</v>
+        <v>20200816U1720WS</v>
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.25">
@@ -2824,10 +2846,10 @@
         <v>20200816</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D62">
         <v>0</v>
@@ -2847,11 +2869,11 @@
       <c r="I62" s="1"/>
       <c r="K62" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20200816U1720ME</v>
+        <v>20200816OBMF</v>
       </c>
       <c r="L62" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20200816U1720WE</v>
+        <v>20200816OBWF</v>
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.25">
@@ -2859,10 +2881,10 @@
         <v>20200816</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D63">
         <v>0</v>
@@ -2871,7 +2893,7 @@
         <v>1</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G63" s="1" t="s">
         <v>43</v>
@@ -2882,22 +2904,22 @@
       <c r="I63" s="1"/>
       <c r="K63" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20200816OBMS</v>
+        <v>20200816U1720ME</v>
       </c>
       <c r="L63" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20200816OBWS</v>
+        <v>20200816U1720WE</v>
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>20200913</v>
+        <v>20200816</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D64">
         <v>0</v>
@@ -2906,10 +2928,10 @@
         <v>1</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="H64" s="1" t="s">
         <v>19</v>
@@ -2917,11 +2939,11 @@
       <c r="I64" s="1"/>
       <c r="K64" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20200913U13BE</v>
+        <v>20200816OBMS</v>
       </c>
       <c r="L64" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20200913U13GE</v>
+        <v>20200816OBWS</v>
       </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.25">
@@ -2929,10 +2951,10 @@
         <v>20200913</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D65">
         <v>0</v>
@@ -2949,14 +2971,16 @@
       <c r="H65" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I65" s="1"/>
+      <c r="I65" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="K65" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20200913U15MF</v>
+        <v>20200913U13BE</v>
       </c>
       <c r="L65" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20200913U15WF</v>
+        <v>20200913U13GE</v>
       </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.25">
@@ -2964,7 +2988,7 @@
         <v>20200913</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>11</v>
@@ -2976,10 +3000,10 @@
         <v>1</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H66" s="1" t="s">
         <v>19</v>
@@ -2987,11 +3011,11 @@
       <c r="I66" s="1"/>
       <c r="K66" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20200913U11BF</v>
+        <v>20200913U15MF</v>
       </c>
       <c r="L66" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20200913U11GF</v>
+        <v>20200913U15WF</v>
       </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.25">
@@ -3002,7 +3026,7 @@
         <v>20</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D67">
         <v>0</v>
@@ -3011,10 +3035,10 @@
         <v>1</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="H67" s="1" t="s">
         <v>19</v>
@@ -3022,11 +3046,11 @@
       <c r="I67" s="1"/>
       <c r="K67" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20200913U11BE</v>
+        <v>20200913U11BF</v>
       </c>
       <c r="L67" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20200913U11GE</v>
+        <v>20200913U11GF</v>
       </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.25">
@@ -3034,10 +3058,10 @@
         <v>20200913</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D68">
         <v>0</v>
@@ -3057,11 +3081,11 @@
       <c r="I68" s="1"/>
       <c r="K68" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20200913U13BF</v>
+        <v>20200913U11BE</v>
       </c>
       <c r="L68" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20200913U13GF</v>
+        <v>20200913U11GE</v>
       </c>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.25">
@@ -3069,10 +3093,10 @@
         <v>20200913</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D69">
         <v>0</v>
@@ -3081,10 +3105,10 @@
         <v>1</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="H69" s="1" t="s">
         <v>19</v>
@@ -3092,19 +3116,19 @@
       <c r="I69" s="1"/>
       <c r="K69" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20200913U15ME</v>
+        <v>20200913U13BF</v>
       </c>
       <c r="L69" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20200913U15WE</v>
+        <v>20200913U13GF</v>
       </c>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>20200920</v>
+        <v>20200913</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>12</v>
@@ -3116,22 +3140,22 @@
         <v>1</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="H70" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="I70" s="1"/>
       <c r="K70" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20200920OME</v>
+        <v>20200913U15ME</v>
       </c>
       <c r="L70" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20200920OWE</v>
+        <v>20200913U15WE</v>
       </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.25">
@@ -3142,7 +3166,7 @@
         <v>18</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D71">
         <v>0</v>
@@ -3151,22 +3175,24 @@
         <v>1</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="H71" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I71" s="1"/>
+      <c r="I71" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="K71" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20200920OMS</v>
+        <v>20200920OME</v>
       </c>
       <c r="L71" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20200920OWS</v>
+        <v>20200920OWE</v>
       </c>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.25">
@@ -3174,10 +3200,10 @@
         <v>20200920</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D72">
         <v>0</v>
@@ -3197,11 +3223,11 @@
       <c r="I72" s="1"/>
       <c r="K72" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20200920VMF</v>
+        <v>20200920OMS</v>
       </c>
       <c r="L72" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20200920VWF</v>
+        <v>20200920OWS</v>
       </c>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.25">
@@ -3209,7 +3235,7 @@
         <v>20200920</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>11</v>
@@ -3221,10 +3247,10 @@
         <v>1</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H73" s="1" t="s">
         <v>26</v>
@@ -3232,11 +3258,11 @@
       <c r="I73" s="1"/>
       <c r="K73" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20200920OMF</v>
+        <v>20200920VMF</v>
       </c>
       <c r="L73" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20200920OWF</v>
+        <v>20200920VWF</v>
       </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.25">
@@ -3244,10 +3270,10 @@
         <v>20200920</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D74">
         <v>0</v>
@@ -3267,11 +3293,11 @@
       <c r="I74" s="1"/>
       <c r="K74" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20200920VME</v>
+        <v>20200920OMF</v>
       </c>
       <c r="L74" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20200920VWE</v>
+        <v>20200920OWF</v>
       </c>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.25">
@@ -3282,7 +3308,7 @@
         <v>9</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D75">
         <v>0</v>
@@ -3302,22 +3328,22 @@
       <c r="I75" s="1"/>
       <c r="K75" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20200920VMS</v>
+        <v>20200920VME</v>
       </c>
       <c r="L75" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20200920VWS</v>
+        <v>20200920VWE</v>
       </c>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>20201018</v>
+        <v>20200920</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D76">
         <v>0</v>
@@ -3326,10 +3352,10 @@
         <v>1</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="H76" s="1" t="s">
         <v>26</v>
@@ -3337,11 +3363,11 @@
       <c r="I76" s="1"/>
       <c r="K76" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20201018U13BE</v>
+        <v>20200920VMS</v>
       </c>
       <c r="L76" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20201018U13GE</v>
+        <v>20200920VWS</v>
       </c>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.25">
@@ -3349,10 +3375,10 @@
         <v>20201018</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D77">
         <v>0</v>
@@ -3369,14 +3395,16 @@
       <c r="H77" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I77" s="1"/>
+      <c r="I77" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="K77" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20201018U15MF</v>
+        <v>20201018U13BE</v>
       </c>
       <c r="L77" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20201018U15WF</v>
+        <v>20201018U13GE</v>
       </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.25">
@@ -3384,7 +3412,7 @@
         <v>20201018</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>11</v>
@@ -3396,10 +3424,10 @@
         <v>1</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H78" s="1" t="s">
         <v>26</v>
@@ -3407,11 +3435,11 @@
       <c r="I78" s="1"/>
       <c r="K78" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20201018U11BF</v>
+        <v>20201018U15MF</v>
       </c>
       <c r="L78" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20201018U11GF</v>
+        <v>20201018U15WF</v>
       </c>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.25">
@@ -3422,7 +3450,7 @@
         <v>20</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D79">
         <v>0</v>
@@ -3431,10 +3459,10 @@
         <v>1</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="H79" s="1" t="s">
         <v>26</v>
@@ -3442,11 +3470,11 @@
       <c r="I79" s="1"/>
       <c r="K79" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20201018U11BE</v>
+        <v>20201018U11BF</v>
       </c>
       <c r="L79" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20201018U11GE</v>
+        <v>20201018U11GF</v>
       </c>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.25">
@@ -3454,10 +3482,10 @@
         <v>20201018</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D80">
         <v>0</v>
@@ -3477,11 +3505,11 @@
       <c r="I80" s="1"/>
       <c r="K80" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20201018U13BF</v>
+        <v>20201018U11BE</v>
       </c>
       <c r="L80" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20201018U13GF</v>
+        <v>20201018U11GE</v>
       </c>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.25">
@@ -3489,10 +3517,10 @@
         <v>20201018</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D81">
         <v>0</v>
@@ -3501,10 +3529,10 @@
         <v>1</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="H81" s="1" t="s">
         <v>26</v>
@@ -3512,22 +3540,22 @@
       <c r="I81" s="1"/>
       <c r="K81" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20201018U15ME</v>
+        <v>20201018U13BF</v>
       </c>
       <c r="L81" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20201018U15WE</v>
+        <v>20201018U13GF</v>
       </c>
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>20201025</v>
+        <v>20201018</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D82">
         <v>0</v>
@@ -3536,10 +3564,10 @@
         <v>1</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="H82" s="1" t="s">
         <v>26</v>
@@ -3547,11 +3575,11 @@
       <c r="I82" s="1"/>
       <c r="K82" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20201025U1720MF</v>
+        <v>20201018U15ME</v>
       </c>
       <c r="L82" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20201025U1720WF</v>
+        <v>20201018U15WE</v>
       </c>
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.25">
@@ -3559,10 +3587,10 @@
         <v>20201025</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D83">
         <v>0</v>
@@ -3571,22 +3599,24 @@
         <v>1</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H83" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I83" s="1"/>
+      <c r="I83" s="1" t="s">
+        <v>53</v>
+      </c>
       <c r="K83" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20201025OBME</v>
+        <v>20201025U1720MF</v>
       </c>
       <c r="L83" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20201025OBWE</v>
+        <v>20201025U1720WF</v>
       </c>
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.25">
@@ -3594,10 +3624,10 @@
         <v>20201025</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D84">
         <v>0</v>
@@ -3606,10 +3636,10 @@
         <v>1</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H84" s="1" t="s">
         <v>26</v>
@@ -3617,11 +3647,11 @@
       <c r="I84" s="1"/>
       <c r="K84" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20201025U1720MS</v>
+        <v>20201025OBME</v>
       </c>
       <c r="L84" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20201025U1720WS</v>
+        <v>20201025OBWE</v>
       </c>
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.25">
@@ -3629,10 +3659,10 @@
         <v>20201025</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D85">
         <v>0</v>
@@ -3641,10 +3671,10 @@
         <v>1</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H85" s="1" t="s">
         <v>26</v>
@@ -3652,11 +3682,11 @@
       <c r="I85" s="1"/>
       <c r="K85" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20201025OBMF</v>
+        <v>20201025U1720MS</v>
       </c>
       <c r="L85" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20201025OBWF</v>
+        <v>20201025U1720WS</v>
       </c>
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.25">
@@ -3664,10 +3694,10 @@
         <v>20201025</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D86">
         <v>0</v>
@@ -3687,11 +3717,11 @@
       <c r="I86" s="1"/>
       <c r="K86" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20201025U1720ME</v>
+        <v>20201025OBMF</v>
       </c>
       <c r="L86" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20201025U1720WE</v>
+        <v>20201025OBWF</v>
       </c>
     </row>
     <row r="87" spans="1:12" x14ac:dyDescent="0.25">
@@ -3699,10 +3729,10 @@
         <v>20201025</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D87">
         <v>0</v>
@@ -3711,7 +3741,7 @@
         <v>1</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G87" s="1" t="s">
         <v>43</v>
@@ -3722,22 +3752,22 @@
       <c r="I87" s="1"/>
       <c r="K87" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20201025OBMS</v>
+        <v>20201025U1720ME</v>
       </c>
       <c r="L87" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20201025OBWS</v>
+        <v>20201025U1720WE</v>
       </c>
     </row>
     <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A88">
-        <v>20201108</v>
+        <v>20201025</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D88">
         <v>0</v>
@@ -3746,22 +3776,22 @@
         <v>1</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="H88" s="1" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="I88" s="1"/>
       <c r="K88" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20201108OME</v>
+        <v>20201025OBMS</v>
       </c>
       <c r="L88" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20201108OWE</v>
+        <v>20201025OBWS</v>
       </c>
     </row>
     <row r="89" spans="1:12" x14ac:dyDescent="0.25">
@@ -3772,7 +3802,7 @@
         <v>18</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D89">
         <v>0</v>
@@ -3781,22 +3811,24 @@
         <v>1</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G89" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="H89" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I89" s="1"/>
+        <v>22</v>
+      </c>
+      <c r="I89" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="K89" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20201108OMS</v>
+        <v>20201108OME</v>
       </c>
       <c r="L89" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20201108OWS</v>
+        <v>20201108OWE</v>
       </c>
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.25">
@@ -3804,10 +3836,10 @@
         <v>20201108</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D90">
         <v>0</v>
@@ -3822,16 +3854,16 @@
         <v>45</v>
       </c>
       <c r="H90" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="I90" s="1"/>
       <c r="K90" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20201108VMF</v>
+        <v>20201108OMS</v>
       </c>
       <c r="L90" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20201108VWF</v>
+        <v>20201108OWS</v>
       </c>
     </row>
     <row r="91" spans="1:12" x14ac:dyDescent="0.25">
@@ -3839,7 +3871,7 @@
         <v>20201108</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="C91" s="1" t="s">
         <v>11</v>
@@ -3851,10 +3883,10 @@
         <v>1</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G91" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H91" s="1" t="s">
         <v>19</v>
@@ -3862,11 +3894,11 @@
       <c r="I91" s="1"/>
       <c r="K91" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20201108OMF</v>
+        <v>20201108VMF</v>
       </c>
       <c r="L91" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20201108OWF</v>
+        <v>20201108VWF</v>
       </c>
     </row>
     <row r="92" spans="1:12" x14ac:dyDescent="0.25">
@@ -3874,10 +3906,10 @@
         <v>20201108</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D92">
         <v>0</v>
@@ -3892,16 +3924,16 @@
         <v>46</v>
       </c>
       <c r="H92" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="I92" s="1"/>
       <c r="K92" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20201108VME</v>
+        <v>20201108OMF</v>
       </c>
       <c r="L92" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20201108VWE</v>
+        <v>20201108OWF</v>
       </c>
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.25">
@@ -3912,7 +3944,7 @@
         <v>9</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D93">
         <v>0</v>
@@ -3932,22 +3964,22 @@
       <c r="I93" s="1"/>
       <c r="K93" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20201108VMS</v>
+        <v>20201108VME</v>
       </c>
       <c r="L93" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20201108VWS</v>
+        <v>20201108VWE</v>
       </c>
     </row>
     <row r="94" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A94">
-        <v>20201115</v>
+        <v>20201108</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>48</v>
+        <v>9</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D94">
         <v>0</v>
@@ -3956,10 +3988,10 @@
         <v>1</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="G94" s="1" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="H94" s="1" t="s">
         <v>19</v>
@@ -3967,11 +3999,11 @@
       <c r="I94" s="1"/>
       <c r="K94" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20201115OTME</v>
+        <v>20201108VMS</v>
       </c>
       <c r="L94" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20201115OTWE</v>
+        <v>20201108VWS</v>
       </c>
     </row>
     <row r="95" spans="1:12" x14ac:dyDescent="0.25">
@@ -3982,7 +4014,7 @@
         <v>48</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D95">
         <v>0</v>
@@ -3991,10 +4023,10 @@
         <v>1</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G95" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H95" s="1" t="s">
         <v>19</v>
@@ -4002,11 +4034,11 @@
       <c r="I95" s="1"/>
       <c r="K95" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20201115OTMS</v>
+        <v>20201115OTME</v>
       </c>
       <c r="L95" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20201115OTWS</v>
+        <v>20201115OTWE</v>
       </c>
     </row>
     <row r="96" spans="1:12" x14ac:dyDescent="0.25">
@@ -4017,7 +4049,7 @@
         <v>48</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D96">
         <v>0</v>
@@ -4026,10 +4058,10 @@
         <v>1</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G96" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H96" s="1" t="s">
         <v>19</v>
@@ -4037,9 +4069,44 @@
       <c r="I96" s="1"/>
       <c r="K96" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
+        <v>20201115OTMS</v>
+      </c>
+      <c r="L96" t="str">
+        <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
+        <v>20201115OTWS</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>20201115</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D97">
+        <v>0</v>
+      </c>
+      <c r="E97">
+        <v>1</v>
+      </c>
+      <c r="F97" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G97" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H97" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I97" s="1"/>
+      <c r="K97" t="str">
+        <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
         <v>20201115OTMF</v>
       </c>
-      <c r="L96" t="str">
+      <c r="L97" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
         <v>20201115OTWF</v>
       </c>

</xml_diff>

<commit_message>
Update for Schools League
</commit_message>
<xml_diff>
--- a/2020/2020FSAdates.xlsx
+++ b/2020/2020FSAdates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rober\Dropbox\Competitions\2020\Results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robert.thomas\Dropbox\Competitions\2020\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48813679-3970-4FEE-B8EB-E4DFA657A989}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D8B4143-6337-495F-9DC2-8A288B97C736}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-12465" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="55">
   <si>
     <t>Date</t>
   </si>
@@ -206,9 +206,6 @@
   </si>
   <si>
     <t>40285</t>
-  </si>
-  <si>
-    <t>U17T</t>
   </si>
 </sst>
 </file>
@@ -663,25 +660,25 @@
   <dimension ref="A1:L103"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="A67" sqref="A67"/>
+      <selection activeCell="B72" sqref="B72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.26953125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.453125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.1796875" customWidth="1"/>
+    <col min="11" max="11" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -716,7 +713,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>20200301</v>
       </c>
@@ -753,7 +750,7 @@
         <v>20200301U13GE</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>20200301</v>
       </c>
@@ -790,7 +787,7 @@
         <v>20200301U15WF</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>20200301</v>
       </c>
@@ -827,7 +824,7 @@
         <v>20200301U11GF</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>20200301</v>
       </c>
@@ -864,7 +861,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>20200301</v>
       </c>
@@ -901,7 +898,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>20200301</v>
       </c>
@@ -938,7 +935,7 @@
         <v>20200301U15WE</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>20200315</v>
       </c>
@@ -975,7 +972,7 @@
         <v>20200315OWE</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>20200315</v>
       </c>
@@ -1012,7 +1009,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>20200315</v>
       </c>
@@ -1049,7 +1046,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>20200315</v>
       </c>
@@ -1086,7 +1083,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>20200315</v>
       </c>
@@ -1123,7 +1120,7 @@
         <v>20200315OWF</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>20200315</v>
       </c>
@@ -1160,7 +1157,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>20200315</v>
       </c>
@@ -1197,7 +1194,7 @@
         <v>20200315VWE</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>20200315</v>
       </c>
@@ -1234,7 +1231,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>20200328</v>
       </c>
@@ -1269,7 +1266,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>20200328</v>
       </c>
@@ -1304,7 +1301,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>20200328</v>
       </c>
@@ -1339,7 +1336,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>20200328</v>
       </c>
@@ -1374,7 +1371,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>20200329</v>
       </c>
@@ -1409,7 +1406,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20200329</v>
       </c>
@@ -1444,7 +1441,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20200329</v>
       </c>
@@ -1479,7 +1476,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>20200329</v>
       </c>
@@ -1514,7 +1511,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>20200329</v>
       </c>
@@ -1549,7 +1546,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>20200503</v>
       </c>
@@ -1584,7 +1581,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>20200503</v>
       </c>
@@ -1619,7 +1616,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>20200503</v>
       </c>
@@ -1654,7 +1651,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>20200503</v>
       </c>
@@ -1689,7 +1686,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>20200503</v>
       </c>
@@ -1724,7 +1721,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>20200503</v>
       </c>
@@ -1759,7 +1756,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>20200517</v>
       </c>
@@ -1794,7 +1791,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>20200517</v>
       </c>
@@ -1829,7 +1826,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>20200517</v>
       </c>
@@ -1864,7 +1861,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>20200517</v>
       </c>
@@ -1899,7 +1896,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>20200517</v>
       </c>
@@ -1934,7 +1931,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>20200517</v>
       </c>
@@ -1969,7 +1966,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>20200524</v>
       </c>
@@ -2004,7 +2001,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>20200524</v>
       </c>
@@ -2039,7 +2036,7 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>20200524</v>
       </c>
@@ -2074,7 +2071,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>20200524</v>
       </c>
@@ -2109,7 +2106,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>20200524</v>
       </c>
@@ -2144,7 +2141,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>20200524</v>
       </c>
@@ -2179,7 +2176,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>20200621</v>
       </c>
@@ -2214,7 +2211,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>20200621</v>
       </c>
@@ -2249,7 +2246,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>20200621</v>
       </c>
@@ -2284,7 +2281,7 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>20200621</v>
       </c>
@@ -2319,7 +2316,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>20200621</v>
       </c>
@@ -2354,7 +2351,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>20200621</v>
       </c>
@@ -2389,7 +2386,7 @@
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>20200628</v>
       </c>
@@ -2424,7 +2421,7 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>20200628</v>
       </c>
@@ -2459,7 +2456,7 @@
         <v/>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>20200628</v>
       </c>
@@ -2494,7 +2491,7 @@
         <v/>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>20200726</v>
       </c>
@@ -2529,7 +2526,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>20200726</v>
       </c>
@@ -2564,7 +2561,7 @@
         <v>20200726OWE</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>20200726</v>
       </c>
@@ -2599,7 +2596,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>20200726</v>
       </c>
@@ -2634,7 +2631,7 @@
         <v/>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>20200726</v>
       </c>
@@ -2669,7 +2666,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>20200726</v>
       </c>
@@ -2704,7 +2701,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>20200726</v>
       </c>
@@ -2739,7 +2736,7 @@
         <v/>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>20200816</v>
       </c>
@@ -2776,7 +2773,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>20200816</v>
       </c>
@@ -2811,7 +2808,7 @@
         <v>20200816U1720WF</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>20200816</v>
       </c>
@@ -2846,7 +2843,7 @@
         <v>20200816OBWE</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>20200816</v>
       </c>
@@ -2881,7 +2878,7 @@
         <v/>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>20200816</v>
       </c>
@@ -2916,7 +2913,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>20200816</v>
       </c>
@@ -2951,7 +2948,7 @@
         <v>20200816OBWF</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>20200816</v>
       </c>
@@ -2986,7 +2983,7 @@
         <v/>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>20200816</v>
       </c>
@@ -3021,7 +3018,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>20200913</v>
       </c>
@@ -3058,7 +3055,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>20200913</v>
       </c>
@@ -3093,7 +3090,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>20200913</v>
       </c>
@@ -3128,7 +3125,7 @@
         <v>20200913U15WF</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>20200913</v>
       </c>
@@ -3163,7 +3160,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>20200913</v>
       </c>
@@ -3198,12 +3195,12 @@
         <v>20200913U11GF</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>20200913</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>11</v>
@@ -3226,14 +3223,14 @@
       <c r="I72" s="1"/>
       <c r="K72" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20200913U17TF</v>
+        <v>20200913U20TF</v>
       </c>
       <c r="L72" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
         <v>N/A</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>20200913</v>
       </c>
@@ -3268,7 +3265,7 @@
         <v/>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>20200913</v>
       </c>
@@ -3303,7 +3300,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>20200913</v>
       </c>
@@ -3338,7 +3335,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>20200913</v>
       </c>
@@ -3373,7 +3370,7 @@
         <v>20200913U15WE</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>20200920</v>
       </c>
@@ -3410,7 +3407,7 @@
         <v>20200920OWE</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>20200920</v>
       </c>
@@ -3445,7 +3442,7 @@
         <v>20200920OWS</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>20200920</v>
       </c>
@@ -3480,7 +3477,7 @@
         <v>20200920VWF</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>20200920</v>
       </c>
@@ -3515,7 +3512,7 @@
         <v>20200920OWF</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>20200920</v>
       </c>
@@ -3550,7 +3547,7 @@
         <v>20200920VWE</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>20200920</v>
       </c>
@@ -3585,7 +3582,7 @@
         <v>20200920VWS</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>20201018</v>
       </c>
@@ -3622,7 +3619,7 @@
         <v>20201018U13GE</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>20201018</v>
       </c>
@@ -3657,7 +3654,7 @@
         <v>20201018U15WF</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>20201018</v>
       </c>
@@ -3692,7 +3689,7 @@
         <v>20201018U11GF</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>20201018</v>
       </c>
@@ -3727,7 +3724,7 @@
         <v>20201018U11GE</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>20201018</v>
       </c>
@@ -3762,7 +3759,7 @@
         <v>20201018U13GF</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>20201018</v>
       </c>
@@ -3797,7 +3794,7 @@
         <v>20201018U15WE</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>20201025</v>
       </c>
@@ -3834,7 +3831,7 @@
         <v>20201025U1720WF</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>20201025</v>
       </c>
@@ -3869,7 +3866,7 @@
         <v>20201025OBWE</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>20201025</v>
       </c>
@@ -3904,7 +3901,7 @@
         <v>20201025U1720WS</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>20201025</v>
       </c>
@@ -3939,7 +3936,7 @@
         <v>20201025OBWF</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>20201025</v>
       </c>
@@ -3974,7 +3971,7 @@
         <v>20201025U1720WE</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>20201025</v>
       </c>
@@ -4009,7 +4006,7 @@
         <v>20201025OBWS</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>20201108</v>
       </c>
@@ -4046,7 +4043,7 @@
         <v>20201108OWE</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>20201108</v>
       </c>
@@ -4081,7 +4078,7 @@
         <v>20201108OWS</v>
       </c>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>20201108</v>
       </c>
@@ -4116,7 +4113,7 @@
         <v>20201108VWF</v>
       </c>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>20201108</v>
       </c>
@@ -4151,7 +4148,7 @@
         <v>20201108OWF</v>
       </c>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>20201108</v>
       </c>
@@ -4186,7 +4183,7 @@
         <v>20201108VWE</v>
       </c>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>20201108</v>
       </c>
@@ -4221,7 +4218,7 @@
         <v>20201108VWS</v>
       </c>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>20201115</v>
       </c>
@@ -4256,7 +4253,7 @@
         <v>20201115OTWE</v>
       </c>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>20201115</v>
       </c>
@@ -4291,7 +4288,7 @@
         <v>20201115OTWS</v>
       </c>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>20201115</v>
       </c>

</xml_diff>

<commit_message>
Update to Dates for Schools
</commit_message>
<xml_diff>
--- a/2020/2020FSAdates.xlsx
+++ b/2020/2020FSAdates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robert.thomas\Dropbox\Competitions\2020\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D8B4143-6337-495F-9DC2-8A288B97C736}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{443627E3-CFDA-4F16-A105-1FBB68333F83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-12465" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="56">
   <si>
     <t>Date</t>
   </si>
@@ -206,6 +206,9 @@
   </si>
   <si>
     <t>40285</t>
+  </si>
+  <si>
+    <t>U17T</t>
   </si>
 </sst>
 </file>
@@ -660,7 +663,7 @@
   <dimension ref="A1:L103"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="B72" sqref="B72"/>
+      <selection activeCell="A72" sqref="A72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3200,7 +3203,7 @@
         <v>20200913</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>11</v>
@@ -3223,7 +3226,7 @@
       <c r="I72" s="1"/>
       <c r="K72" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20200913U20TF</v>
+        <v>20200913U17TF</v>
       </c>
       <c r="L72" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>

</xml_diff>

<commit_message>
Remove links for entry
</commit_message>
<xml_diff>
--- a/2020/2020FSAdates.xlsx
+++ b/2020/2020FSAdates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robert.thomas\Dropbox\Competitions\2020\Results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rober\Dropbox\Competitions\2020\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{443627E3-CFDA-4F16-A105-1FBB68333F83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98FBD904-7085-415B-B06D-0CD957D37923}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-12465" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="50">
   <si>
     <t>Date</t>
   </si>
@@ -188,24 +188,6 @@
   </si>
   <si>
     <t>OT</t>
-  </si>
-  <si>
-    <t>40255</t>
-  </si>
-  <si>
-    <t>40256</t>
-  </si>
-  <si>
-    <t>40257</t>
-  </si>
-  <si>
-    <t>40258</t>
-  </si>
-  <si>
-    <t>40284</t>
-  </si>
-  <si>
-    <t>40285</t>
   </si>
   <si>
     <t>U17T</t>
@@ -324,11 +306,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:I103" tableType="xml" totalsRowShown="0" connectionId="2">
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I103">
-    <sortCondition ref="A2:A103"/>
-    <sortCondition ref="F2:F103"/>
-    <sortCondition ref="B2:B103"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:I106" tableType="xml" totalsRowShown="0" connectionId="2">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I106">
+    <sortCondition ref="A2:A106"/>
+    <sortCondition ref="F2:F106"/>
+    <sortCondition ref="B2:B106"/>
   </sortState>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="Date" name="Date">
@@ -660,28 +642,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L103"/>
+  <dimension ref="A1:L106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="A72" sqref="A72"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.26953125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.140625" customWidth="1"/>
+    <col min="11" max="11" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -716,7 +696,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>20200301</v>
       </c>
@@ -741,9 +721,7 @@
       <c r="H2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="3">
-        <v>37513</v>
-      </c>
+      <c r="I2" s="3"/>
       <c r="K2" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
         <v>20200301U13BE</v>
@@ -753,7 +731,7 @@
         <v>20200301U13GE</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>20200301</v>
       </c>
@@ -778,9 +756,7 @@
       <c r="H3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="3">
-        <v>37513</v>
-      </c>
+      <c r="I3" s="3"/>
       <c r="K3" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
         <v>20200301U15MF</v>
@@ -790,7 +766,7 @@
         <v>20200301U15WF</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>20200301</v>
       </c>
@@ -815,9 +791,7 @@
       <c r="H4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I4" s="3">
-        <v>37513</v>
-      </c>
+      <c r="I4" s="3"/>
       <c r="K4" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
         <v>20200301U11BF</v>
@@ -827,7 +801,7 @@
         <v>20200301U11GF</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>20200301</v>
       </c>
@@ -852,9 +826,7 @@
       <c r="H5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I5" s="3">
-        <v>37513</v>
-      </c>
+      <c r="I5" s="3"/>
       <c r="K5" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
         <v>20200301U11E</v>
@@ -864,7 +836,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>20200301</v>
       </c>
@@ -889,9 +861,7 @@
       <c r="H6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I6" s="3">
-        <v>37513</v>
-      </c>
+      <c r="I6" s="3"/>
       <c r="K6" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
         <v>20200301U13F</v>
@@ -901,7 +871,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>20200301</v>
       </c>
@@ -926,9 +896,7 @@
       <c r="H7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I7" s="3">
-        <v>37513</v>
-      </c>
+      <c r="I7" s="3"/>
       <c r="K7" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
         <v>20200301U15ME</v>
@@ -938,7 +906,7 @@
         <v>20200301U15WE</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>20200315</v>
       </c>
@@ -963,9 +931,7 @@
       <c r="H8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I8" s="3">
-        <v>37514</v>
-      </c>
+      <c r="I8" s="3"/>
       <c r="K8" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
         <v>20200315OME</v>
@@ -975,7 +941,7 @@
         <v>20200315OWE</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>20200315</v>
       </c>
@@ -1000,9 +966,7 @@
       <c r="H9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I9" s="3">
-        <v>37514</v>
-      </c>
+      <c r="I9" s="3"/>
       <c r="K9" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
         <v>20200315OS</v>
@@ -1012,7 +976,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>20200315</v>
       </c>
@@ -1037,9 +1001,7 @@
       <c r="H10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I10" s="3">
-        <v>37514</v>
-      </c>
+      <c r="I10" s="3"/>
       <c r="K10" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
         <v>N/A</v>
@@ -1049,7 +1011,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>20200315</v>
       </c>
@@ -1074,9 +1036,7 @@
       <c r="H11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I11" s="3">
-        <v>37514</v>
-      </c>
+      <c r="I11" s="3"/>
       <c r="K11" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
         <v>20200315OF</v>
@@ -1086,7 +1046,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>20200315</v>
       </c>
@@ -1111,9 +1071,7 @@
       <c r="H12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I12" s="3">
-        <v>37514</v>
-      </c>
+      <c r="I12" s="3"/>
       <c r="K12" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
         <v>20200315OMF</v>
@@ -1123,7 +1081,7 @@
         <v>20200315OWF</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>20200315</v>
       </c>
@@ -1148,9 +1106,7 @@
       <c r="H13" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I13" s="3">
-        <v>37514</v>
-      </c>
+      <c r="I13" s="3"/>
       <c r="K13" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
         <v>20200315VE</v>
@@ -1160,7 +1116,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>20200315</v>
       </c>
@@ -1185,9 +1141,7 @@
       <c r="H14" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I14" s="3">
-        <v>37514</v>
-      </c>
+      <c r="I14" s="3"/>
       <c r="K14" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
         <v>20200315VME</v>
@@ -1197,7 +1151,7 @@
         <v>20200315VWE</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>20200315</v>
       </c>
@@ -1222,9 +1176,7 @@
       <c r="H15" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I15" s="3">
-        <v>37514</v>
-      </c>
+      <c r="I15" s="3"/>
       <c r="K15" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
         <v>N/A</v>
@@ -1234,7 +1186,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>20200328</v>
       </c>
@@ -1269,7 +1221,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>20200328</v>
       </c>
@@ -1304,7 +1256,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>20200328</v>
       </c>
@@ -1339,7 +1291,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>20200328</v>
       </c>
@@ -1374,7 +1326,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>20200329</v>
       </c>
@@ -1409,7 +1361,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20200329</v>
       </c>
@@ -1444,7 +1396,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>20200329</v>
       </c>
@@ -1479,7 +1431,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>20200329</v>
       </c>
@@ -1514,7 +1466,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>20200329</v>
       </c>
@@ -1549,7 +1501,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>20200503</v>
       </c>
@@ -1584,7 +1536,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>20200503</v>
       </c>
@@ -1619,7 +1571,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>20200503</v>
       </c>
@@ -1654,7 +1606,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>20200503</v>
       </c>
@@ -1689,7 +1641,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>20200503</v>
       </c>
@@ -1724,7 +1676,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>20200503</v>
       </c>
@@ -1759,7 +1711,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>20200517</v>
       </c>
@@ -1794,7 +1746,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>20200517</v>
       </c>
@@ -1829,7 +1781,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>20200517</v>
       </c>
@@ -1864,7 +1816,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>20200517</v>
       </c>
@@ -1899,7 +1851,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>20200517</v>
       </c>
@@ -1934,7 +1886,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>20200517</v>
       </c>
@@ -1969,7 +1921,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>20200524</v>
       </c>
@@ -2004,7 +1956,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>20200524</v>
       </c>
@@ -2039,7 +1991,7 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>20200524</v>
       </c>
@@ -2074,7 +2026,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>20200524</v>
       </c>
@@ -2109,7 +2061,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>20200524</v>
       </c>
@@ -2144,7 +2096,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>20200524</v>
       </c>
@@ -2179,7 +2131,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>20200621</v>
       </c>
@@ -2214,7 +2166,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>20200621</v>
       </c>
@@ -2249,7 +2201,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>20200621</v>
       </c>
@@ -2284,7 +2236,7 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>20200621</v>
       </c>
@@ -2319,7 +2271,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>20200621</v>
       </c>
@@ -2354,7 +2306,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>20200621</v>
       </c>
@@ -2389,7 +2341,7 @@
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>20200628</v>
       </c>
@@ -2424,7 +2376,7 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>20200628</v>
       </c>
@@ -2459,7 +2411,7 @@
         <v/>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>20200628</v>
       </c>
@@ -2494,7 +2446,7 @@
         <v/>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>20200726</v>
       </c>
@@ -2529,7 +2481,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>20200726</v>
       </c>
@@ -2564,7 +2516,7 @@
         <v>20200726OWE</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>20200726</v>
       </c>
@@ -2599,7 +2551,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>20200726</v>
       </c>
@@ -2634,7 +2586,7 @@
         <v/>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>20200726</v>
       </c>
@@ -2669,7 +2621,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>20200726</v>
       </c>
@@ -2704,7 +2656,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>20200726</v>
       </c>
@@ -2739,7 +2691,7 @@
         <v/>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>20200816</v>
       </c>
@@ -2764,9 +2716,7 @@
       <c r="H59" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I59" s="1" t="s">
-        <v>49</v>
-      </c>
+      <c r="I59" s="1"/>
       <c r="K59" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
         <v>20200816U1720F</v>
@@ -2776,7 +2726,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>20200816</v>
       </c>
@@ -2811,7 +2761,7 @@
         <v>20200816U1720WF</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>20200816</v>
       </c>
@@ -2846,7 +2796,7 @@
         <v>20200816OBWE</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>20200816</v>
       </c>
@@ -2881,7 +2831,7 @@
         <v/>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>20200816</v>
       </c>
@@ -2916,7 +2866,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>20200816</v>
       </c>
@@ -2951,7 +2901,7 @@
         <v>20200816OBWF</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>20200816</v>
       </c>
@@ -2986,7 +2936,7 @@
         <v/>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>20200816</v>
       </c>
@@ -3021,7 +2971,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>20200913</v>
       </c>
@@ -3046,9 +2996,7 @@
       <c r="H67" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I67" s="1" t="s">
-        <v>50</v>
-      </c>
+      <c r="I67" s="1"/>
       <c r="K67" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
         <v>20200913U13E</v>
@@ -3058,7 +3006,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>20200913</v>
       </c>
@@ -3093,7 +3041,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>20200913</v>
       </c>
@@ -3128,7 +3076,7 @@
         <v>20200913U15WF</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>20200913</v>
       </c>
@@ -3163,7 +3111,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>20200913</v>
       </c>
@@ -3198,12 +3146,12 @@
         <v>20200913U11GF</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>20200913</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>11</v>
@@ -3233,7 +3181,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>20200913</v>
       </c>
@@ -3268,7 +3216,7 @@
         <v/>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>20200913</v>
       </c>
@@ -3303,7 +3251,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>20200913</v>
       </c>
@@ -3338,7 +3286,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>20200913</v>
       </c>
@@ -3373,7 +3321,7 @@
         <v>20200913U15WE</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>20200920</v>
       </c>
@@ -3387,7 +3335,7 @@
         <v>0</v>
       </c>
       <c r="E77">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F77" s="1" t="s">
         <v>32</v>
@@ -3398,19 +3346,17 @@
       <c r="H77" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I77" s="1" t="s">
-        <v>51</v>
-      </c>
+      <c r="I77" s="1"/>
       <c r="K77" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20200920OME</v>
+        <v>20200920OE</v>
       </c>
       <c r="L77" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20200920OWE</v>
-      </c>
-    </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+        <v>N/A</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>20200920</v>
       </c>
@@ -3418,7 +3364,7 @@
         <v>18</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D78">
         <v>0</v>
@@ -3427,10 +3373,10 @@
         <v>1</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="H78" s="1" t="s">
         <v>26</v>
@@ -3438,28 +3384,28 @@
       <c r="I78" s="1"/>
       <c r="K78" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20200920OMS</v>
+        <v>20200920OME</v>
       </c>
       <c r="L78" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20200920OWS</v>
-      </c>
-    </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+        <v>20200920OWE</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>20200920</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D79">
         <v>0</v>
       </c>
       <c r="E79">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F79" s="1" t="s">
         <v>37</v>
@@ -3473,34 +3419,34 @@
       <c r="I79" s="1"/>
       <c r="K79" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20200920VMF</v>
+        <v>20200920OS</v>
       </c>
       <c r="L79" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20200920VWF</v>
-      </c>
-    </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+        <v>N/A</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>20200920</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D80">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E80">
         <v>1</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H80" s="1" t="s">
         <v>26</v>
@@ -3508,28 +3454,28 @@
       <c r="I80" s="1"/>
       <c r="K80" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20200920OMF</v>
+        <v>N/A</v>
       </c>
       <c r="L80" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20200920OWF</v>
-      </c>
-    </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+        <v/>
+      </c>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>20200920</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D81">
         <v>0</v>
       </c>
       <c r="E81">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F81" s="1" t="s">
         <v>38</v>
@@ -3543,22 +3489,22 @@
       <c r="I81" s="1"/>
       <c r="K81" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20200920VME</v>
+        <v>20200920OF</v>
       </c>
       <c r="L81" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20200920VWE</v>
-      </c>
-    </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+        <v>N/A</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>20200920</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D82">
         <v>0</v>
@@ -3578,19 +3524,19 @@
       <c r="I82" s="1"/>
       <c r="K82" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20200920VMS</v>
+        <v>20200920OMF</v>
       </c>
       <c r="L82" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20200920VWS</v>
-      </c>
-    </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+        <v>20200920OWF</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A83">
-        <v>20201018</v>
+        <v>20200920</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>12</v>
@@ -3599,38 +3545,36 @@
         <v>0</v>
       </c>
       <c r="E83">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="H83" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I83" s="1" t="s">
-        <v>52</v>
-      </c>
+      <c r="I83" s="1"/>
       <c r="K83" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20201018U13BE</v>
+        <v>20200920VE</v>
       </c>
       <c r="L83" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20201018U13GE</v>
-      </c>
-    </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+        <v>N/A</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A84">
-        <v>20201018</v>
+        <v>20200920</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D84">
         <v>0</v>
@@ -3639,10 +3583,10 @@
         <v>1</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="H84" s="1" t="s">
         <v>26</v>
@@ -3650,34 +3594,34 @@
       <c r="I84" s="1"/>
       <c r="K84" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20201018U15MF</v>
+        <v>20200920VME</v>
       </c>
       <c r="L84" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20201018U15WF</v>
-      </c>
-    </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+        <v>20200920VWE</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A85">
-        <v>20201018</v>
+        <v>20200920</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D85">
         <v>0</v>
       </c>
       <c r="E85">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="H85" s="1" t="s">
         <v>26</v>
@@ -3685,19 +3629,19 @@
       <c r="I85" s="1"/>
       <c r="K85" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20201018U11BF</v>
+        <v>20200920VS</v>
       </c>
       <c r="L85" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20201018U11GF</v>
-      </c>
-    </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+        <v>N/A</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>20201018</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>12</v>
@@ -3709,10 +3653,10 @@
         <v>1</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="H86" s="1" t="s">
         <v>26</v>
@@ -3720,19 +3664,19 @@
       <c r="I86" s="1"/>
       <c r="K86" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20201018U11BE</v>
+        <v>20201018U13BE</v>
       </c>
       <c r="L86" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20201018U11GE</v>
-      </c>
-    </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+        <v>20201018U13GE</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>20201018</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>11</v>
@@ -3744,10 +3688,10 @@
         <v>1</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="G87" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="H87" s="1" t="s">
         <v>26</v>
@@ -3755,22 +3699,22 @@
       <c r="I87" s="1"/>
       <c r="K87" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20201018U13BF</v>
+        <v>20201018U15MF</v>
       </c>
       <c r="L87" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20201018U13GF</v>
-      </c>
-    </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+        <v>20201018U15WF</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>20201018</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D88">
         <v>0</v>
@@ -3779,10 +3723,10 @@
         <v>1</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H88" s="1" t="s">
         <v>26</v>
@@ -3790,22 +3734,22 @@
       <c r="I88" s="1"/>
       <c r="K88" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20201018U15ME</v>
+        <v>20201018U11BF</v>
       </c>
       <c r="L88" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20201018U15WE</v>
-      </c>
-    </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+        <v>20201018U11GF</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A89">
-        <v>20201025</v>
+        <v>20201018</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D89">
         <v>0</v>
@@ -3814,35 +3758,33 @@
         <v>1</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="G89" s="1" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="H89" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I89" s="1" t="s">
-        <v>53</v>
-      </c>
+      <c r="I89" s="1"/>
       <c r="K89" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20201025U1720MF</v>
+        <v>20201018U11BE</v>
       </c>
       <c r="L89" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20201025U1720WF</v>
-      </c>
-    </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+        <v>20201018U11GE</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A90">
-        <v>20201025</v>
+        <v>20201018</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D90">
         <v>0</v>
@@ -3851,10 +3793,10 @@
         <v>1</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="G90" s="1" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="H90" s="1" t="s">
         <v>26</v>
@@ -3862,22 +3804,22 @@
       <c r="I90" s="1"/>
       <c r="K90" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20201025OBME</v>
+        <v>20201018U13BF</v>
       </c>
       <c r="L90" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20201025OBWE</v>
-      </c>
-    </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+        <v>20201018U13GF</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A91">
-        <v>20201025</v>
+        <v>20201018</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D91">
         <v>0</v>
@@ -3886,10 +3828,10 @@
         <v>1</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G91" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H91" s="1" t="s">
         <v>26</v>
@@ -3897,19 +3839,19 @@
       <c r="I91" s="1"/>
       <c r="K91" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20201025U1720MS</v>
+        <v>20201018U15ME</v>
       </c>
       <c r="L91" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20201025U1720WS</v>
-      </c>
-    </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+        <v>20201018U15WE</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>20201025</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>11</v>
@@ -3921,10 +3863,10 @@
         <v>1</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G92" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H92" s="1" t="s">
         <v>26</v>
@@ -3932,19 +3874,19 @@
       <c r="I92" s="1"/>
       <c r="K92" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20201025OBMF</v>
+        <v>20201025U1720MF</v>
       </c>
       <c r="L92" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20201025OBWF</v>
-      </c>
-    </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+        <v>20201025U1720WF</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>20201025</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>12</v>
@@ -3956,10 +3898,10 @@
         <v>1</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G93" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H93" s="1" t="s">
         <v>26</v>
@@ -3967,19 +3909,19 @@
       <c r="I93" s="1"/>
       <c r="K93" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20201025U1720ME</v>
+        <v>20201025OBME</v>
       </c>
       <c r="L93" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20201025U1720WE</v>
-      </c>
-    </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+        <v>20201025OBWE</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A94">
         <v>20201025</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>13</v>
@@ -3991,10 +3933,10 @@
         <v>1</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G94" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H94" s="1" t="s">
         <v>26</v>
@@ -4002,60 +3944,58 @@
       <c r="I94" s="1"/>
       <c r="K94" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20201025OBMS</v>
+        <v>20201025U1720MS</v>
       </c>
       <c r="L94" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20201025OBWS</v>
-      </c>
-    </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+        <v>20201025U1720WS</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A95">
-        <v>20201108</v>
+        <v>20201025</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C95" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D95">
+        <v>0</v>
+      </c>
+      <c r="E95">
+        <v>1</v>
+      </c>
+      <c r="F95" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G95" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H95" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I95" s="1"/>
+      <c r="K95" t="str">
+        <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
+        <v>20201025OBMF</v>
+      </c>
+      <c r="L95" t="str">
+        <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
+        <v>20201025OBWF</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A96">
+        <v>20201025</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C96" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D95">
-        <v>0</v>
-      </c>
-      <c r="E95">
-        <v>1</v>
-      </c>
-      <c r="F95" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G95" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="H95" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I95" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="K95" t="str">
-        <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20201108OME</v>
-      </c>
-      <c r="L95" t="str">
-        <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20201108OWE</v>
-      </c>
-    </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A96">
-        <v>20201108</v>
-      </c>
-      <c r="B96" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C96" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="D96">
         <v>0</v>
       </c>
@@ -4063,33 +4003,33 @@
         <v>1</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G96" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H96" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="I96" s="1"/>
       <c r="K96" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20201108OMS</v>
+        <v>20201025U1720ME</v>
       </c>
       <c r="L96" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20201108OWS</v>
-      </c>
-    </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
+        <v>20201025U1720WE</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A97">
-        <v>20201108</v>
+        <v>20201025</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D97">
         <v>0</v>
@@ -4098,25 +4038,25 @@
         <v>1</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G97" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H97" s="1" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="I97" s="1"/>
       <c r="K97" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20201108VMF</v>
+        <v>20201025OBMS</v>
       </c>
       <c r="L97" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20201108VWF</v>
-      </c>
-    </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
+        <v>20201025OBWS</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A98">
         <v>20201108</v>
       </c>
@@ -4124,7 +4064,7 @@
         <v>18</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D98">
         <v>0</v>
@@ -4133,33 +4073,33 @@
         <v>1</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="G98" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="H98" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="I98" s="1"/>
       <c r="K98" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20201108OMF</v>
+        <v>20201108OME</v>
       </c>
       <c r="L98" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20201108OWF</v>
-      </c>
-    </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
+        <v>20201108OWE</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A99">
         <v>20201108</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D99">
         <v>0</v>
@@ -4168,25 +4108,25 @@
         <v>1</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G99" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H99" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="I99" s="1"/>
       <c r="K99" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20201108VME</v>
+        <v>20201108OMS</v>
       </c>
       <c r="L99" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20201108VWE</v>
-      </c>
-    </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
+        <v>20201108OWS</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A100">
         <v>20201108</v>
       </c>
@@ -4194,7 +4134,7 @@
         <v>9</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D100">
         <v>0</v>
@@ -4203,10 +4143,10 @@
         <v>1</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G100" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H100" s="1" t="s">
         <v>19</v>
@@ -4214,22 +4154,22 @@
       <c r="I100" s="1"/>
       <c r="K100" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20201108VMS</v>
+        <v>20201108VMF</v>
       </c>
       <c r="L100" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20201108VWS</v>
-      </c>
-    </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
+        <v>20201108VWF</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A101">
-        <v>20201115</v>
+        <v>20201108</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D101">
         <v>0</v>
@@ -4238,33 +4178,33 @@
         <v>1</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="G101" s="1" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="H101" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="I101" s="1"/>
       <c r="K101" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20201115OTME</v>
+        <v>20201108OMF</v>
       </c>
       <c r="L101" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20201115OTWE</v>
-      </c>
-    </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
+        <v>20201108OWF</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A102">
-        <v>20201115</v>
+        <v>20201108</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>48</v>
+        <v>9</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D102">
         <v>0</v>
@@ -4273,10 +4213,10 @@
         <v>1</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G102" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="H102" s="1" t="s">
         <v>19</v>
@@ -4284,22 +4224,22 @@
       <c r="I102" s="1"/>
       <c r="K102" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20201115OTMS</v>
+        <v>20201108VME</v>
       </c>
       <c r="L102" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20201115OTWS</v>
-      </c>
-    </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
+        <v>20201108VWE</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A103">
-        <v>20201115</v>
+        <v>20201108</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>48</v>
+        <v>9</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D103">
         <v>0</v>
@@ -4311,7 +4251,7 @@
         <v>38</v>
       </c>
       <c r="G103" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="H103" s="1" t="s">
         <v>19</v>
@@ -4319,9 +4259,114 @@
       <c r="I103" s="1"/>
       <c r="K103" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
+        <v>20201108VMS</v>
+      </c>
+      <c r="L103" t="str">
+        <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
+        <v>20201108VWS</v>
+      </c>
+    </row>
+    <row r="104" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A104">
+        <v>20201115</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D104">
+        <v>0</v>
+      </c>
+      <c r="E104">
+        <v>1</v>
+      </c>
+      <c r="F104" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G104" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H104" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I104" s="1"/>
+      <c r="K104" t="str">
+        <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
+        <v>20201115OTME</v>
+      </c>
+      <c r="L104" t="str">
+        <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
+        <v>20201115OTWE</v>
+      </c>
+    </row>
+    <row r="105" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A105">
+        <v>20201115</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D105">
+        <v>0</v>
+      </c>
+      <c r="E105">
+        <v>1</v>
+      </c>
+      <c r="F105" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G105" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H105" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I105" s="1"/>
+      <c r="K105" t="str">
+        <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
+        <v>20201115OTMS</v>
+      </c>
+      <c r="L105" t="str">
+        <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
+        <v>20201115OTWS</v>
+      </c>
+    </row>
+    <row r="106" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A106">
+        <v>20201115</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D106">
+        <v>0</v>
+      </c>
+      <c r="E106">
+        <v>1</v>
+      </c>
+      <c r="F106" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G106" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H106" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I106" s="1"/>
+      <c r="K106" t="str">
+        <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
         <v>20201115OTMF</v>
       </c>
-      <c r="L103" t="str">
+      <c r="L106" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
         <v>20201115OTWF</v>
       </c>

</xml_diff>

<commit_message>
ReUpload new dates for italian relay
</commit_message>
<xml_diff>
--- a/2020/2020FSAdates.xlsx
+++ b/2020/2020FSAdates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rober\Dropbox\Competitions\2020\Results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robert.thomas\Dropbox\Competitions\2020\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98FBD904-7085-415B-B06D-0CD957D37923}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA40208C-0316-4A4C-9C7A-679D136D10BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="51">
   <si>
     <t>Date</t>
   </si>
@@ -191,6 +191,9 @@
   </si>
   <si>
     <t>U17T</t>
+  </si>
+  <si>
+    <t>U13T</t>
   </si>
 </sst>
 </file>
@@ -306,7 +309,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:I106" tableType="xml" totalsRowShown="0" connectionId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:I108" tableType="xml" totalsRowShown="0" connectionId="2">
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I106">
     <sortCondition ref="A2:A106"/>
     <sortCondition ref="F2:F106"/>
@@ -642,26 +645,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L106"/>
+  <dimension ref="A1:L108"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="A104" sqref="A104"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.26953125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.453125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.1796875" customWidth="1"/>
+    <col min="11" max="11" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -696,7 +701,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>20200301</v>
       </c>
@@ -731,7 +736,7 @@
         <v>20200301U13GE</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>20200301</v>
       </c>
@@ -766,7 +771,7 @@
         <v>20200301U15WF</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>20200301</v>
       </c>
@@ -801,7 +806,7 @@
         <v>20200301U11GF</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>20200301</v>
       </c>
@@ -836,7 +841,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>20200301</v>
       </c>
@@ -871,7 +876,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>20200301</v>
       </c>
@@ -906,7 +911,7 @@
         <v>20200301U15WE</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>20200315</v>
       </c>
@@ -941,7 +946,7 @@
         <v>20200315OWE</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>20200315</v>
       </c>
@@ -976,7 +981,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>20200315</v>
       </c>
@@ -1011,7 +1016,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>20200315</v>
       </c>
@@ -1046,7 +1051,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>20200315</v>
       </c>
@@ -1081,7 +1086,7 @@
         <v>20200315OWF</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>20200315</v>
       </c>
@@ -1116,7 +1121,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>20200315</v>
       </c>
@@ -1151,7 +1156,7 @@
         <v>20200315VWE</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>20200315</v>
       </c>
@@ -1186,7 +1191,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>20200328</v>
       </c>
@@ -1221,7 +1226,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>20200328</v>
       </c>
@@ -1256,7 +1261,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>20200328</v>
       </c>
@@ -1291,7 +1296,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>20200328</v>
       </c>
@@ -1326,7 +1331,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>20200329</v>
       </c>
@@ -1361,7 +1366,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20200329</v>
       </c>
@@ -1396,7 +1401,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20200329</v>
       </c>
@@ -1431,7 +1436,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>20200329</v>
       </c>
@@ -1466,7 +1471,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>20200329</v>
       </c>
@@ -1501,7 +1506,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>20200503</v>
       </c>
@@ -1536,7 +1541,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>20200503</v>
       </c>
@@ -1571,7 +1576,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>20200503</v>
       </c>
@@ -1606,7 +1611,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>20200503</v>
       </c>
@@ -1641,7 +1646,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>20200503</v>
       </c>
@@ -1676,7 +1681,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>20200503</v>
       </c>
@@ -1711,7 +1716,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>20200517</v>
       </c>
@@ -1746,7 +1751,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>20200517</v>
       </c>
@@ -1781,7 +1786,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>20200517</v>
       </c>
@@ -1816,7 +1821,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>20200517</v>
       </c>
@@ -1851,7 +1856,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>20200517</v>
       </c>
@@ -1886,7 +1891,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>20200517</v>
       </c>
@@ -1921,7 +1926,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>20200524</v>
       </c>
@@ -1956,7 +1961,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>20200524</v>
       </c>
@@ -1991,7 +1996,7 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>20200524</v>
       </c>
@@ -2026,7 +2031,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>20200524</v>
       </c>
@@ -2061,7 +2066,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>20200524</v>
       </c>
@@ -2096,7 +2101,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>20200524</v>
       </c>
@@ -2131,7 +2136,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>20200621</v>
       </c>
@@ -2166,7 +2171,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>20200621</v>
       </c>
@@ -2201,7 +2206,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>20200621</v>
       </c>
@@ -2236,7 +2241,7 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>20200621</v>
       </c>
@@ -2271,7 +2276,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>20200621</v>
       </c>
@@ -2306,7 +2311,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>20200621</v>
       </c>
@@ -2341,7 +2346,7 @@
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>20200628</v>
       </c>
@@ -2376,7 +2381,7 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>20200628</v>
       </c>
@@ -2411,7 +2416,7 @@
         <v/>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>20200628</v>
       </c>
@@ -2446,7 +2451,7 @@
         <v/>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>20200726</v>
       </c>
@@ -2481,7 +2486,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>20200726</v>
       </c>
@@ -2516,7 +2521,7 @@
         <v>20200726OWE</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>20200726</v>
       </c>
@@ -2551,7 +2556,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>20200726</v>
       </c>
@@ -2586,7 +2591,7 @@
         <v/>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>20200726</v>
       </c>
@@ -2621,7 +2626,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>20200726</v>
       </c>
@@ -2656,7 +2661,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>20200726</v>
       </c>
@@ -2691,7 +2696,7 @@
         <v/>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>20200816</v>
       </c>
@@ -2726,7 +2731,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>20200816</v>
       </c>
@@ -2761,7 +2766,7 @@
         <v>20200816U1720WF</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>20200816</v>
       </c>
@@ -2796,7 +2801,7 @@
         <v>20200816OBWE</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>20200816</v>
       </c>
@@ -2831,7 +2836,7 @@
         <v/>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>20200816</v>
       </c>
@@ -2866,7 +2871,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>20200816</v>
       </c>
@@ -2901,7 +2906,7 @@
         <v>20200816OBWF</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>20200816</v>
       </c>
@@ -2936,7 +2941,7 @@
         <v/>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>20200816</v>
       </c>
@@ -2971,7 +2976,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>20200913</v>
       </c>
@@ -3006,7 +3011,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>20200913</v>
       </c>
@@ -3041,7 +3046,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>20200913</v>
       </c>
@@ -3076,7 +3081,7 @@
         <v>20200913U15WF</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>20200913</v>
       </c>
@@ -3111,7 +3116,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>20200913</v>
       </c>
@@ -3146,7 +3151,7 @@
         <v>20200913U11GF</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>20200913</v>
       </c>
@@ -3181,7 +3186,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>20200913</v>
       </c>
@@ -3216,7 +3221,7 @@
         <v/>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>20200913</v>
       </c>
@@ -3251,7 +3256,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>20200913</v>
       </c>
@@ -3286,7 +3291,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>20200913</v>
       </c>
@@ -3321,7 +3326,7 @@
         <v>20200913U15WE</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>20200920</v>
       </c>
@@ -3356,7 +3361,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>20200920</v>
       </c>
@@ -3391,7 +3396,7 @@
         <v>20200920OWE</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>20200920</v>
       </c>
@@ -3426,7 +3431,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>20200920</v>
       </c>
@@ -3461,7 +3466,7 @@
         <v/>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>20200920</v>
       </c>
@@ -3496,7 +3501,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>20200920</v>
       </c>
@@ -3531,7 +3536,7 @@
         <v>20200920OWF</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>20200920</v>
       </c>
@@ -3566,7 +3571,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>20200920</v>
       </c>
@@ -3601,7 +3606,7 @@
         <v>20200920VWE</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>20200920</v>
       </c>
@@ -3636,7 +3641,7 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>20201018</v>
       </c>
@@ -3671,7 +3676,7 @@
         <v>20201018U13GE</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>20201018</v>
       </c>
@@ -3706,7 +3711,7 @@
         <v>20201018U15WF</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>20201018</v>
       </c>
@@ -3741,7 +3746,7 @@
         <v>20201018U11GF</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>20201018</v>
       </c>
@@ -3776,7 +3781,7 @@
         <v>20201018U11GE</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>20201018</v>
       </c>
@@ -3811,7 +3816,7 @@
         <v>20201018U13GF</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>20201018</v>
       </c>
@@ -3846,7 +3851,7 @@
         <v>20201018U15WE</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>20201025</v>
       </c>
@@ -3881,7 +3886,7 @@
         <v>20201025U1720WF</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>20201025</v>
       </c>
@@ -3916,7 +3921,7 @@
         <v>20201025OBWE</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>20201025</v>
       </c>
@@ -3951,7 +3956,7 @@
         <v>20201025U1720WS</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>20201025</v>
       </c>
@@ -3986,7 +3991,7 @@
         <v>20201025OBWF</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>20201025</v>
       </c>
@@ -4021,7 +4026,7 @@
         <v>20201025U1720WE</v>
       </c>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>20201025</v>
       </c>
@@ -4056,7 +4061,7 @@
         <v>20201025OBWS</v>
       </c>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>20201108</v>
       </c>
@@ -4091,7 +4096,7 @@
         <v>20201108OWE</v>
       </c>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>20201108</v>
       </c>
@@ -4126,7 +4131,7 @@
         <v>20201108OWS</v>
       </c>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>20201108</v>
       </c>
@@ -4161,7 +4166,7 @@
         <v>20201108VWF</v>
       </c>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>20201108</v>
       </c>
@@ -4196,7 +4201,7 @@
         <v>20201108OWF</v>
       </c>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>20201108</v>
       </c>
@@ -4231,7 +4236,7 @@
         <v>20201108VWE</v>
       </c>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>20201108</v>
       </c>
@@ -4266,7 +4271,7 @@
         <v>20201108VWS</v>
       </c>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>20201115</v>
       </c>
@@ -4280,7 +4285,7 @@
         <v>0</v>
       </c>
       <c r="E104">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F104" s="1" t="s">
         <v>32</v>
@@ -4294,34 +4299,34 @@
       <c r="I104" s="1"/>
       <c r="K104" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20201115OTME</v>
+        <v>20201115OTE</v>
       </c>
       <c r="L104" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20201115OTWE</v>
-      </c>
-    </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.35">
+        <v>N/A</v>
+      </c>
+    </row>
+    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>20201115</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D105">
         <v>0</v>
       </c>
       <c r="E105">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G105" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H105" s="1" t="s">
         <v>19</v>
@@ -4329,34 +4334,34 @@
       <c r="I105" s="1"/>
       <c r="K105" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20201115OTMS</v>
+        <v>20201115U17TF</v>
       </c>
       <c r="L105" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20201115OTWS</v>
-      </c>
-    </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.35">
+        <v>N/A</v>
+      </c>
+    </row>
+    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>20201115</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D106">
         <v>0</v>
       </c>
       <c r="E106">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="G106" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H106" s="1" t="s">
         <v>19</v>
@@ -4364,11 +4369,81 @@
       <c r="I106" s="1"/>
       <c r="K106" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20201115OTMF</v>
+        <v>20201115U17TE</v>
       </c>
       <c r="L106" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>20201115OTWF</v>
+        <v>N/A</v>
+      </c>
+    </row>
+    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>20201115</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D107">
+        <v>0</v>
+      </c>
+      <c r="E107">
+        <v>0</v>
+      </c>
+      <c r="F107" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G107" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H107" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I107" s="1"/>
+      <c r="K107" t="str">
+        <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
+        <v>20201115U13TF</v>
+      </c>
+      <c r="L107" t="str">
+        <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
+        <v>N/A</v>
+      </c>
+    </row>
+    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>20201115</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D108">
+        <v>0</v>
+      </c>
+      <c r="E108">
+        <v>0</v>
+      </c>
+      <c r="F108" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G108" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H108" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I108" s="1"/>
+      <c r="K108" t="str">
+        <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
+        <v>20201115U13TE</v>
+      </c>
+      <c r="L108" t="str">
+        <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
+        <v>N/A</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Dates for Teams
</commit_message>
<xml_diff>
--- a/2020/2020FSAdates.xlsx
+++ b/2020/2020FSAdates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FSA\Dropbox\Competitions\2020\Results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robert.thomas\Dropbox\Competitions\2020\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F66BBAF5-36AD-42F2-A23E-305D7A56A962}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAE83DB7-11E1-45A5-87F3-4CF94BFAD53A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2445" yWindow="1485" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="51">
   <si>
     <t>Date</t>
   </si>
@@ -647,8 +647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="D105" sqref="D105"/>
+    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
+      <selection activeCell="C113" sqref="C113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4593,9 +4593,7 @@
       <c r="B113" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C113" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="C113" s="1"/>
       <c r="D113">
         <v>0</v>
       </c>
@@ -4614,7 +4612,7 @@
       <c r="I113" s="1"/>
       <c r="K113" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20201115OTE</v>
+        <v>20201115OT</v>
       </c>
       <c r="L113" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>

</xml_diff>

<commit_message>
20201115 Update Results for U17TF
</commit_message>
<xml_diff>
--- a/2020/2020FSAdates.xlsx
+++ b/2020/2020FSAdates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FSA\Dropbox\Competitions\2020\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E91F4394-3978-437E-8644-1589A225D3D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C702B8BE-691E-4EDE-8FFC-0CEDBE9EC114}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -648,7 +648,7 @@
   <dimension ref="A1:L119"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
-      <selection activeCell="D118" sqref="D118"/>
+      <selection activeCell="A116" sqref="A116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4700,7 +4700,7 @@
         <v>11</v>
       </c>
       <c r="D116">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E116">
         <v>0</v>
@@ -4717,11 +4717,11 @@
       <c r="I116" s="1"/>
       <c r="K116" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>N/A</v>
+        <v>20201115U17TF</v>
       </c>
       <c r="L116" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v/>
+        <v>N/A</v>
       </c>
     </row>
     <row r="117" spans="1:12" x14ac:dyDescent="0.25">
@@ -4735,7 +4735,7 @@
         <v>12</v>
       </c>
       <c r="D117">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E117">
         <v>0</v>
@@ -4752,11 +4752,11 @@
       <c r="I117" s="1"/>
       <c r="K117" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"B","M"),"")&amp;Table1[[#This Row],[Weapon]])</f>
-        <v>20201115U17TE</v>
+        <v>N/A</v>
       </c>
       <c r="L117" t="str">
         <f>IF(Table1[[#This Row],[Cancelled]]=1,"",IF(Table1[[#This Row],[SplitGender]]=0,"N/A",Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Category]]&amp;IF(Table1[[#This Row],[SplitGender]]=1,IF(OR(Table1[[#This Row],[Category]]="U9",Table1[[#This Row],[Category]]="U11",Table1[[#This Row],[Category]]="U13"),"G","W"),"")&amp;Table1[[#This Row],[Weapon]]))</f>
-        <v>N/A</v>
+        <v/>
       </c>
     </row>
     <row r="118" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>